<commit_message>
do the structure change for tenant and unit - leaseagrm next
</commit_message>
<xml_diff>
--- a/excel_templates/unit-template.xlsx
+++ b/excel_templates/unit-template.xlsx
@@ -12,47 +12,80 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="apartment" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Number of bedrooms</t>
-  </si>
-  <si>
-    <t>Number of bathroom</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Balcony</t>
   </si>
   <si>
-    <t>Number of windows</t>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Bedroom number</t>
+  </si>
+  <si>
+    <t>Bathroom number</t>
+  </si>
+  <si>
+    <t>Window number</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PKKG02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PKK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 bikes, 1 TV</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Compulsory</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
   <si>
     <t>Area</t>
   </si>
   <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>May Thi Nghe</t>
+    <t xml:space="preserve"> Number (m2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +221,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FF444444"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,19 +425,25 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+      <patternFill patternType="lightUp">
+        <fgColor theme="4"/>
+        <bgColor theme="4" tint="-0.24994659260841701"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -517,6 +573,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -562,26 +629,33 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="21" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -903,247 +977,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4">
+        <v>84</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>501</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6">
-        <v>132</v>
-      </c>
-      <c r="D2" s="6">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>3</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>